<commit_message>
excel to two dim
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\Brillio\java_selenium_workspace\OpenEmrAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,9 +34,6 @@
     <t>Language</t>
   </si>
   <si>
-    <t>User Name</t>
-  </si>
-  <si>
     <t>Expected Error</t>
   </si>
   <si>
@@ -60,6 +59,9 @@
   </si>
   <si>
     <t>Paul</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -380,7 +382,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +395,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -402,52 +404,76 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
invalid credential with excel connect
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Password</t>
   </si>
@@ -49,19 +49,13 @@
     <t>Invalid username or password</t>
   </si>
   <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Peter123</t>
-  </si>
-  <si>
-    <t>Paul123</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>John124</t>
+  </si>
+  <si>
+    <t>Kign</t>
   </si>
 </sst>
 </file>
@@ -379,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +389,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -423,7 +417,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -432,20 +426,6 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel - common dataprovider
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
     <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="addPatientTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Password</t>
   </si>
@@ -92,6 +92,45 @@
   </si>
   <si>
     <t>accountant</t>
+  </si>
+  <si>
+    <t>Lanaguage</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>ExpectedValue</t>
+  </si>
+  <si>
+    <t>2022-06-02</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>John Wick</t>
+  </si>
+  <si>
+    <t>Wick</t>
+  </si>
+  <si>
+    <t>Expected Alert Text</t>
+  </si>
+  <si>
+    <t>Tobacco</t>
   </si>
 </sst>
 </file>
@@ -127,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,12 +658,114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>